<commit_message>
Added code for H2H resolution
</commit_message>
<xml_diff>
--- a/2013-2014Teams.xlsx
+++ b/2013-2014Teams.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Grade</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Girls</t>
+  </si>
+  <si>
+    <t>XTM</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,11 +143,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +179,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,15 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,8 +545,11 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -572,7 +595,7 @@
       </c>
       <c r="P2" s="6"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -618,7 +641,7 @@
       </c>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -664,7 +687,7 @@
       </c>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -710,7 +733,7 @@
       </c>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -724,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6">
         <v>2</v>
@@ -760,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -800,7 +823,7 @@
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -846,7 +869,7 @@
       </c>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -892,7 +915,7 @@
       </c>
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -938,7 +961,7 @@
       </c>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -974,11 +997,14 @@
         <v>1</v>
       </c>
       <c r="O11" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1024,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>8</v>
       </c>
@@ -1061,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" s="7">
         <v>1</v>

</xml_diff>